<commit_message>
Add new and update existing materials list spreadsheets
Added 20251120-material-list-to-buy.xlsx and updated material-list-to-buy.xlsx in the materials list directory to reflect the latest changes in required materials.
</commit_message>
<xml_diff>
--- a/design/20251107-materials-list/material-list-to-buy.xlsx
+++ b/design/20251107-materials-list/material-list-to-buy.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Suresh\git\ars-sigrama\design\20251107-materials-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E3EAB9-5914-4E6A-9E28-E50D7D404721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F9EC43-F4C9-452D-BD1B-C779472A9C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{53F401F1-5CA7-40B8-B77C-197E3E3C70EF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{53F401F1-5CA7-40B8-B77C-197E3E3C70EF}"/>
   </bookViews>
   <sheets>
     <sheet name="old" sheetId="1" r:id="rId1"/>
-    <sheet name="20251114" sheetId="2" r:id="rId2"/>
+    <sheet name="20251114-required" sheetId="2" r:id="rId2"/>
+    <sheet name="20251114-optional" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="153">
   <si>
     <t>Sl No</t>
   </si>
@@ -272,29 +273,260 @@
     <t>Unit price (USD)</t>
   </si>
   <si>
-    <t>M9 Male cable connector, Contacts: 2, 4.0-5.0 mm, unshielded, solder, IP40</t>
-  </si>
-  <si>
-    <t>M9 Female panel mount connector, Contacts: 2, unshielded, solder, IP40, M9x0,5, Front mounting</t>
-  </si>
-  <si>
-    <t>09 0074 00 02</t>
-  </si>
-  <si>
-    <t>99 0071 102 02</t>
-  </si>
-  <si>
     <t>Connector on the panel side</t>
   </si>
   <si>
     <t>Connector on the sensor side</t>
+  </si>
+  <si>
+    <t>SC1113</t>
+  </si>
+  <si>
+    <t>Computadoras de placa simple Raspberry Pi 5/16GB</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 5</t>
+  </si>
+  <si>
+    <t>Main computer:
+1. Accessing SSD
+2. User Interface
+3. Implementing algorithms</t>
+  </si>
+  <si>
+    <t>Product information</t>
+  </si>
+  <si>
+    <t>https://mou.sr/3LBm9Fv</t>
+  </si>
+  <si>
+    <t>Piezas</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/catalog/specsheets/Raspberry_Pi_5_Single%20Board%20Computer%20(SBC)%20v2%20Data%20Sheet%20dated%209-26-23.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESP32-P4-Function-EV-Board </t>
+  </si>
+  <si>
+    <t>ESP32 P4</t>
+  </si>
+  <si>
+    <t>https://docs.espressif.com/projects/esp-dev-kits/en/latest/esp32p4/esp32-p4-function-ev-board/user_guide.html#esp32-p4-function-ev-board-v1-5-2</t>
+  </si>
+  <si>
+    <t>SC1166</t>
+  </si>
+  <si>
+    <t>HAT-Sombreros/placas complementarias Raspberry Pi M.2 HAT+ for Pi 5</t>
+  </si>
+  <si>
+    <t>Conexion a M2 SSD</t>
+  </si>
+  <si>
+    <t>https://mou.sr/4nY90DJ</t>
+  </si>
+  <si>
+    <t>https://pip-assets.raspberrypi.com/categories/1268-raspberry-pi-m-2-hat-compact/documents/RP-009234-MM-1-Raspberry%20Pi%20M.2%20HAT_%20product%20brief.pdf?disposition=inline</t>
+  </si>
+  <si>
+    <t>Guardar Datos como valores instentanios y ondas, curvas etc</t>
+  </si>
+  <si>
+    <t>Why Optional</t>
+  </si>
+  <si>
+    <t>Tengo una SSD Personal que puedo usar mientras. Pero para producción se necesita de marca buena como Swissbit para clidad de trabajo industriales</t>
+  </si>
+  <si>
+    <t>https://www.analog.com/media/en/technical-documentation/evaluation-documentation/EVAL-AD7616SDZ-Schematics.zip
+https://www.analog.com/en/resources/evaluation-hardware-and-software/evaluation-boards-kits/eval-ad7616.html
+https://www.analog.com/media/en/technical-documentation/data-sheets/AD7616-P.pdf</t>
+  </si>
+  <si>
+    <t>GPS-21834</t>
+  </si>
+  <si>
+    <t>The SAM-M10Q includes a built-in chip antenna and is compatible with the L1 band on all five GNSS constellations</t>
+  </si>
+  <si>
+    <t>SAM-M10Q</t>
+  </si>
+  <si>
+    <t>Medi tiempo, y posicion con precision:
+60 ns en tiempo
+1.5m en logitud</t>
+  </si>
+  <si>
+    <t>https://mou.sr/3K9ZwYa</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/sparkfun-gps-breakout-chip-antenna-sam-m10q-qwiic.html</t>
+  </si>
+  <si>
+    <t>It is required only if we need very high precision in time</t>
+  </si>
+  <si>
+    <t>https://mou.sr/3LVHzNt
+(debe tener una manera de compra interna al sigrama)</t>
+  </si>
+  <si>
+    <t>EGG.0K.303.CLL</t>
+  </si>
+  <si>
+    <t>FGG.0K.303.CLAC50</t>
+  </si>
+  <si>
+    <t>https://mou.sr/3X5r6J5</t>
+  </si>
+  <si>
+    <t>Conectores circulares de presionar y jalar STRAIGHT PLUG MALE W. CABLE COLLET</t>
+  </si>
+  <si>
+    <t>Conectores circulares de presionar y jalar 3P STRAIGHT FEMALE PNL MNT SOLDER</t>
+  </si>
+  <si>
+    <t>https://mou.sr/4pj93v3</t>
+  </si>
+  <si>
+    <t>FGG.0K.303.CLAC50Z</t>
+  </si>
+  <si>
+    <t>https://www.lemo.com/int_en/solutions/originals/k-outdoor-keyed/fgg-0k-303-clac50.html</t>
+  </si>
+  <si>
+    <t>https://www.lemo.com/int_en/solutions/originals/k-outdoor-keyed/egg-0k-303-cll.html</t>
+  </si>
+  <si>
+    <t>Digilent Zybo Z7‑20</t>
+  </si>
+  <si>
+    <t>https://digilent.com/shop/zybo-z7-zynq-7000-arm-fpga-soc-development-board/?srsltid=AfmBOoqB-b7qGqYXPJnd2gFRvSPVmV4eWlRfqFPZVsp86C60ZV_H7w6-</t>
+  </si>
+  <si>
+    <t>Zybo Z7-20</t>
+  </si>
+  <si>
+    <t>The Zybo Z7 is a ready-to-use embedded software and digital circuit development board built around the AMD Zynq™-7000 family. The Zynq-7000 tightly integrates a dual-core ARM Cortex-A9 processor with AMD 7-series Field Programmable Gate Array (FPGA) logic.</t>
+  </si>
+  <si>
+    <t>This can be good idea to implement but design will be complex. May take more time and the results are not very different. However can be used for future projects.</t>
+  </si>
+  <si>
+    <t>Dupont</t>
+  </si>
+  <si>
+    <t>Conexion entre tarjetas</t>
+  </si>
+  <si>
+    <t>AC/ DC TO DC 24-600V TO 12V 24V 2A Buck Converter voltage Regulator switching power supply AC 110V 220V 36V 48V 60V 72V 84V 96V</t>
+  </si>
+  <si>
+    <t>https://es.aliexpress.com/item/1005005624426475.html</t>
+  </si>
+  <si>
+    <t>Convertir 220VAC to 12VDC</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.mx/MLM-705157159-cables-jumpers-dupont-120-pzas-10-cm-proyectos-arduino-_JM#origin%3Dshare%26sid%3Dshare</t>
+  </si>
+  <si>
+    <t>Juego de 120 piezas</t>
+  </si>
+  <si>
+    <t>Electronic components + PCBs</t>
+  </si>
+  <si>
+    <t>To prepare complimentary circuits for 
+1. Current measurement
+2. Voltaje measurement
+3. Inidcator ciruits
+4. Triggering circuits
+5. Power management</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>Elements to consider to prepare a in-house prototype</t>
+  </si>
+  <si>
+    <t>Battery backup unit</t>
+  </si>
+  <si>
+    <t>Enclosure with heat dessipation</t>
+  </si>
+  <si>
+    <t>https://www.raspberrypi.com/products/touch-display-2/</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Touch Display 2 is a touchscreen portrait display for Raspberry Pi. It is ideal for interactive projects such as tablets, entertainment systems, and information dashboards. Available in 5-inch and 7-inch variants from $40.</t>
+  </si>
+  <si>
+    <t>We can prepare a version without touchscreen display</t>
+  </si>
+  <si>
+    <t>5'' Raspberry Pi Touch Display 2</t>
+  </si>
+  <si>
+    <t>https://www.mercadolibre.com.mx/paquete-de-2-baterias-recargables-vapcell-p50-37v-5000mah/p/MLM2048500990?pdp_filters=item_id%3AMLM1901771075#origin%3Dshare%26sid%3Dshare%26wid%3DMLM1901771075</t>
+  </si>
+  <si>
+    <t>Paquete De 2 Baterias Recargables Vapcell P50 3.7v 5000mah</t>
+  </si>
+  <si>
+    <t>Pilas para Autonomia de Analizador</t>
+  </si>
+  <si>
+    <t>1. Interfacing ADC
+2. Interfac to GPS module</t>
+  </si>
+  <si>
+    <t>Pack de 2</t>
+  </si>
+  <si>
+    <t>P50</t>
+  </si>
+  <si>
+    <t>https://www.waveshare.com/ups-hat-e.htm</t>
+  </si>
+  <si>
+    <t>UPS HAT (E) (EN)</t>
+  </si>
+  <si>
+    <t>UPS HAT (E) for Raspberry Pi, Supports 4× 21700 Li batteries (NOT included), Bi-Directional Fast charging, 5V 6A Output, Pogo Pins Connector, Raspberry Pi UPS</t>
+  </si>
+  <si>
+    <t>BMS compatible con Raspberry Pi</t>
+  </si>
+  <si>
+    <t>UPS HAT</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.mx/SAMSUNG-Pro-Endurance-Tarjeta-Memoria/dp/B09WB3D5GQ</t>
+  </si>
+  <si>
+    <t>Samsung Pro Endurance Tarjeta de Memoria MicroSDXC de 256 GB</t>
+  </si>
+  <si>
+    <t>Tarjeta SD para ESP32</t>
+  </si>
+  <si>
+    <t>256GB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +550,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -327,7 +566,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -335,12 +574,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -360,8 +615,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -695,13 +999,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56762CF-59FD-4735-AA09-7439E2CB7D49}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,6 +1277,9 @@
       <c r="C8" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="E8" s="3" t="s">
         <v>51</v>
       </c>
@@ -1093,16 +1403,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>66</v>
@@ -1110,22 +1423,43 @@
       <c r="H12" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="I12" s="3">
+        <v>50</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="3">
+        <v>4</v>
+      </c>
+      <c r="I13" s="3">
+        <v>62</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -1172,6 +1506,8 @@
     <hyperlink ref="L10" r:id="rId23" xr:uid="{93BD0EAD-8A5F-4329-9FDE-AD2E65EF10BC}"/>
     <hyperlink ref="K11" r:id="rId24" xr:uid="{28899A44-F1FB-40F7-8E98-3F1F18204AD0}"/>
     <hyperlink ref="L11" r:id="rId25" xr:uid="{5A11EA1F-21AA-4852-B6FE-7E3E4B02AD48}"/>
+    <hyperlink ref="L13" r:id="rId26" xr:uid="{34294A49-01EC-4462-ADB8-209AE5F2EEC8}"/>
+    <hyperlink ref="L12" r:id="rId27" xr:uid="{576C0EE2-975E-469C-B904-5CFAD9FBDFB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1179,14 +1515,1099 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214198EB-3255-4F6D-B3C1-0933671F7425}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="14"/>
+    <col min="9" max="9" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45" style="3" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>120</v>
+      </c>
+      <c r="I2" s="13">
+        <f>G2*H2</f>
+        <v>120</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <v>12</v>
+      </c>
+      <c r="I3" s="13">
+        <f t="shared" ref="I3:I13" si="0">G3*H3</f>
+        <v>12</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <v>60</v>
+      </c>
+      <c r="I4" s="13">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <v>98.88</v>
+      </c>
+      <c r="I5" s="13">
+        <f t="shared" si="0"/>
+        <v>98.88</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>70</v>
+      </c>
+      <c r="I6" s="13">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="9">
+        <v>72913</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>50</v>
+      </c>
+      <c r="I7" s="13">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="9">
+        <v>72913</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>50</v>
+      </c>
+      <c r="I8" s="13">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="9">
+        <v>4</v>
+      </c>
+      <c r="H9" s="13">
+        <v>170</v>
+      </c>
+      <c r="I9" s="13">
+        <f t="shared" si="0"/>
+        <v>680</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="9">
+        <v>4</v>
+      </c>
+      <c r="H10" s="13">
+        <v>50</v>
+      </c>
+      <c r="I10" s="13">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="9">
+        <v>4</v>
+      </c>
+      <c r="H11" s="13">
+        <v>62</v>
+      </c>
+      <c r="I11" s="13">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="9">
+        <v>3</v>
+      </c>
+      <c r="H12" s="13">
+        <v>4</v>
+      </c>
+      <c r="I12" s="13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="9">
+        <v>1</v>
+      </c>
+      <c r="H13" s="13">
+        <v>10</v>
+      </c>
+      <c r="I13" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" s="9">
+        <v>1</v>
+      </c>
+      <c r="H14" s="13">
+        <v>300</v>
+      </c>
+      <c r="I14" s="13">
+        <f t="shared" ref="I14:I17" si="1">G14*H14</f>
+        <v>300</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="9">
+        <v>1</v>
+      </c>
+      <c r="H15" s="13">
+        <v>35</v>
+      </c>
+      <c r="I15" s="13">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="9">
+        <v>21700</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="9">
+        <v>2</v>
+      </c>
+      <c r="H16" s="13">
+        <v>30</v>
+      </c>
+      <c r="I16" s="13">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="9">
+        <v>1</v>
+      </c>
+      <c r="H17" s="13">
+        <v>30</v>
+      </c>
+      <c r="I17" s="13">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13">
+        <f>SUM(I2:I19)</f>
+        <v>2035.88</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>2</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{9B587626-EFEF-43D1-87E8-C220050E7DF4}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{062701AA-849A-494B-B959-3CD22376AB56}"/>
+    <hyperlink ref="K4" r:id="rId3" xr:uid="{A221B462-1844-4CAB-A065-D026647487D0}"/>
+    <hyperlink ref="J4" r:id="rId4" location="esp32-p4-function-ev-board-v1-5-2" xr:uid="{7BBC8EB5-C020-4BCE-ABB7-B4947922D0E5}"/>
+    <hyperlink ref="K3" r:id="rId5" xr:uid="{B77504AA-AA3D-4152-981A-9C6FCF7B5B37}"/>
+    <hyperlink ref="J3" r:id="rId6" xr:uid="{3BAE2654-094A-4A58-81AF-8792F66DA710}"/>
+    <hyperlink ref="K5" r:id="rId7" xr:uid="{44C7AC65-6A7F-4523-ACD5-D3535FF1EEA4}"/>
+    <hyperlink ref="K6" r:id="rId8" xr:uid="{51B31CDB-9C02-4414-BE86-027072C15BDB}"/>
+    <hyperlink ref="J6" r:id="rId9" xr:uid="{D9714CEE-72B9-4F1D-8FD1-8D9BDEF0F358}"/>
+    <hyperlink ref="J7" r:id="rId10" xr:uid="{B4F141CB-DFAF-4311-AD6F-FFC9CC7E4B53}"/>
+    <hyperlink ref="J8" r:id="rId11" xr:uid="{BB5FF3C0-D003-4C00-9BBD-D757E060DD47}"/>
+    <hyperlink ref="J9" r:id="rId12" xr:uid="{564ABBFB-52A8-44E6-BF48-7FE46D05003D}"/>
+    <hyperlink ref="K7" r:id="rId13" xr:uid="{9831B52D-E2E2-4FFB-892E-0DAD44AFECEA}"/>
+    <hyperlink ref="K8" r:id="rId14" xr:uid="{938A934E-1B72-4D75-B333-F44AF751194B}"/>
+    <hyperlink ref="K9" r:id="rId15" xr:uid="{D1E1F3F5-5EA5-4458-B483-617BF662A044}"/>
+    <hyperlink ref="J11" r:id="rId16" xr:uid="{8AE5093F-D714-49C6-8E7B-EE5364B55412}"/>
+    <hyperlink ref="J10" r:id="rId17" xr:uid="{22C63C0C-A5EC-4B6A-AEA7-16EFBFC466AF}"/>
+    <hyperlink ref="K13" r:id="rId18" xr:uid="{7A4E6CA9-981D-48F1-9BB3-EFA9C5F9FCC4}"/>
+    <hyperlink ref="K12" r:id="rId19" location="origin%3Dshare%26sid%3Dshare" xr:uid="{34B68E16-EB01-4870-B149-865A96488704}"/>
+    <hyperlink ref="K16" r:id="rId20" location="origin%3Dshare%26sid%3Dshare%26wid%3DMLM1901771075" xr:uid="{8BBEAFAE-F304-4B6E-AC37-7F10D5D0E7DF}"/>
+    <hyperlink ref="J15" r:id="rId21" xr:uid="{FC2A106D-2062-4056-A1A0-05B49980EDF2}"/>
+    <hyperlink ref="K17" r:id="rId22" xr:uid="{5C0005C3-C19B-4A57-AC13-9FE1A6E9DD58}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C00B57DC-24D5-4A1C-BD62-D2E1C681B6E1}">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1</v>
+      </c>
+      <c r="H2" s="20">
+        <v>175</v>
+      </c>
+      <c r="I2" s="20">
+        <f t="shared" ref="I2:I14" si="0">G2*H2</f>
+        <v>175</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="20">
+        <v>280</v>
+      </c>
+      <c r="I3" s="20">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1</v>
+      </c>
+      <c r="H4" s="20">
+        <v>96</v>
+      </c>
+      <c r="I4" s="20">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="20">
+        <v>400</v>
+      </c>
+      <c r="I5" s="20">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="20">
+        <v>50</v>
+      </c>
+      <c r="I6" s="20">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="20">
+        <f>SUM(I2:I13)</f>
+        <v>1001</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{FF59431A-2556-4634-93FB-51DD37E32813}"/>
+    <hyperlink ref="K2" r:id="rId2" xr:uid="{E2665F0D-970E-4CAC-8B05-D980037464AA}"/>
+    <hyperlink ref="K3" r:id="rId3" xr:uid="{BB1E6544-DF5D-4CB0-B732-A718B46EF284}"/>
+    <hyperlink ref="K4" r:id="rId4" xr:uid="{DE89AEE4-F076-4B2C-B395-469644AC03B9}"/>
+    <hyperlink ref="J3" r:id="rId5" xr:uid="{22D0B0C5-1A3B-478D-90D3-786C2304EB0F}"/>
+    <hyperlink ref="J4" r:id="rId6" xr:uid="{BA2A3B0A-D7BF-4CF9-AA4C-EFAD5A8CAE4F}"/>
+    <hyperlink ref="J5" r:id="rId7" xr:uid="{C172330F-B50F-4A87-8DF9-F23CD2572B2E}"/>
+    <hyperlink ref="J6" r:id="rId8" xr:uid="{622E1EFE-9AE7-4835-AD34-2D6C59EB66A1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>